<commit_message>
more data from model/simulation
</commit_message>
<xml_diff>
--- a/Experiment/Analysis2.xlsx
+++ b/Experiment/Analysis2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\Documents\2023-FYP\Experiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15198B7A-6F37-4AC6-BED1-0031424F3D9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB55BE0A-BDA3-479F-84A1-E4B26746F043}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{247A1E3C-87D8-467C-B97F-715594754AA3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{247A1E3C-87D8-467C-B97F-715594754AA3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -101,7 +101,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -152,15 +152,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -905,16 +904,16 @@
                   <c:v>0.48</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.65</c:v>
+                  <c:v>0.54</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.76</c:v>
+                  <c:v>0.84</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.5</c:v>
+                  <c:v>0.47</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.57999999999999996</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1704,10 +1703,10 @@
                   <c:v>0.41</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.65</c:v>
+                  <c:v>0.54</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.5</c:v>
+                  <c:v>0.47</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1781,10 +1780,10 @@
                   <c:v>0.48</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.76</c:v>
+                  <c:v>0.84</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.57999999999999996</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5291,8 +5290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4986B364-A491-49A2-9CB8-330D7C5C1208}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5307,28 +5306,28 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C2" s="2">
+      <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2">
         <v>1</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2">
         <v>3</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2">
         <v>3</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2">
         <v>4</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2">
         <v>4</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2">
         <v>6</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2">
         <v>6</v>
       </c>
     </row>
@@ -5359,7 +5358,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
@@ -5391,7 +5390,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+      <c r="A5" s="3"/>
       <c r="B5" t="s">
         <v>11</v>
       </c>
@@ -5407,21 +5406,21 @@
       <c r="F5">
         <v>0.48</v>
       </c>
-      <c r="G5" s="3">
-        <v>0.65</v>
-      </c>
-      <c r="H5" s="3">
-        <v>0.76</v>
-      </c>
-      <c r="I5" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="J5" s="3">
-        <v>0.57999999999999996</v>
+      <c r="G5" s="4">
+        <v>0.54</v>
+      </c>
+      <c r="H5" s="4">
+        <v>0.84</v>
+      </c>
+      <c r="I5" s="4">
+        <v>0.47</v>
+      </c>
+      <c r="J5" s="4">
+        <v>0.6</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
+      <c r="A6" s="3"/>
       <c r="B6" t="s">
         <v>12</v>
       </c>
@@ -5443,31 +5442,31 @@
       <c r="H6">
         <v>0.89</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="1">
         <v>0.52</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="1">
         <v>0.52</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
+      <c r="A8" s="3"/>
       <c r="B8" t="s">
         <v>1</v>
       </c>
@@ -5489,11 +5488,11 @@
       <c r="H8">
         <v>0.85</v>
       </c>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
+      <c r="A9" s="3"/>
       <c r="B9" t="s">
         <v>2</v>
       </c>
@@ -5515,43 +5514,43 @@
       <c r="H9">
         <v>0.95</v>
       </c>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B10" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10">
         <v>0.62</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10">
         <v>0.62</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10">
         <v>0.37</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10">
         <v>0.62</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10">
         <v>0.85</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10">
         <v>1.1299999999999999</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10">
         <v>0.45</v>
       </c>
-      <c r="J10" s="4">
+      <c r="J10">
         <v>0.99</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
+      <c r="A11" s="3"/>
       <c r="B11" t="s">
         <v>1</v>
       </c>
@@ -5573,11 +5572,11 @@
       <c r="H11">
         <v>1.07</v>
       </c>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
+      <c r="A12" s="3"/>
       <c r="B12" t="s">
         <v>2</v>
       </c>
@@ -5599,13 +5598,13 @@
       <c r="H12">
         <v>1.26</v>
       </c>
-      <c r="I12" s="3"/>
+      <c r="I12" s="1"/>
       <c r="J12">
         <v>0.91</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B13" t="s">
@@ -5613,13 +5612,13 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
+      <c r="A14" s="3"/>
       <c r="B14" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
+      <c r="A15" s="3"/>
       <c r="B15" t="s">
         <v>2</v>
       </c>
@@ -5639,9 +5638,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CD0A37E-004E-4ADA-86C5-3C95F5510AAC}">
-  <dimension ref="B1:J14"/>
+  <dimension ref="B1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
@@ -5658,22 +5657,22 @@
       </c>
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C2" s="1">
+      <c r="C2" s="3">
         <v>1</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1">
+      <c r="D2" s="3"/>
+      <c r="E2" s="3">
         <v>3</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1">
+      <c r="F2" s="3"/>
+      <c r="G2" s="3">
         <v>4</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1">
+      <c r="H2" s="3"/>
+      <c r="I2" s="3">
         <v>6</v>
       </c>
-      <c r="J2" s="1"/>
+      <c r="J2" s="3"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
@@ -5746,16 +5745,16 @@
       <c r="F5">
         <v>0.48</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="1">
         <v>0.65</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="1">
         <v>0.76</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="1">
         <v>0.5</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="1">
         <v>0.57999999999999996</v>
       </c>
     </row>
@@ -5781,10 +5780,10 @@
       <c r="H6">
         <v>0.89</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="1">
         <v>0.52</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="1">
         <v>0.52</v>
       </c>
     </row>
@@ -5794,22 +5793,22 @@
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1" t="s">
+      <c r="D10" s="3"/>
+      <c r="E10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1" t="s">
+      <c r="F10" s="3"/>
+      <c r="G10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1" t="s">
+      <c r="H10" s="3"/>
+      <c r="I10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J10" s="1"/>
+      <c r="J10" s="3"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
@@ -5841,35 +5840,35 @@
       <c r="B12" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="2">
         <f>C4/C6-1</f>
         <v>-0.16129032258064513</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="2">
         <f t="shared" ref="D12:J12" si="0">D4/D6-1</f>
         <v>-0.28767123287671226</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="2">
         <f t="shared" si="0"/>
         <v>-0.20512820512820518</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="2">
         <f t="shared" si="0"/>
         <v>0.33333333333333326</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="2">
         <f t="shared" si="0"/>
         <v>-0.19230769230769229</v>
       </c>
-      <c r="H12" s="5">
+      <c r="H12" s="2">
         <f t="shared" si="0"/>
         <v>-0.202247191011236</v>
       </c>
-      <c r="I12" s="5">
+      <c r="I12" s="2">
         <f t="shared" si="0"/>
         <v>-0.30769230769230771</v>
       </c>
-      <c r="J12" s="5">
+      <c r="J12" s="2">
         <f t="shared" si="0"/>
         <v>0.21153846153846145</v>
       </c>
@@ -5878,44 +5877,38 @@
       <c r="B13" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="2">
         <f xml:space="preserve"> C5/C6-1</f>
         <v>-0.14516129032258063</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="2">
         <f t="shared" ref="D13:J13" si="1" xml:space="preserve"> D5/D6-1</f>
         <v>-6.8493150684931448E-2</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="2">
         <f t="shared" si="1"/>
         <v>5.12820512820511E-2</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="2">
         <f t="shared" si="1"/>
         <v>0.23076923076923062</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="2">
         <f t="shared" si="1"/>
         <v>-0.16666666666666663</v>
       </c>
-      <c r="H13" s="5">
+      <c r="H13" s="2">
         <f t="shared" si="1"/>
         <v>-0.1460674157303371</v>
       </c>
-      <c r="I13" s="5">
+      <c r="I13" s="2">
         <f t="shared" si="1"/>
         <v>-3.8461538461538547E-2</v>
       </c>
-      <c r="J13" s="5">
+      <c r="J13" s="2">
         <f t="shared" si="1"/>
         <v>0.1153846153846152</v>
       </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
stage 6 simulation complete
</commit_message>
<xml_diff>
--- a/Experiment/Analysis2.xlsx
+++ b/Experiment/Analysis2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\Documents\2023-FYP\Experiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB55BE0A-BDA3-479F-84A1-E4B26746F043}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D450F5F-8D4E-42F9-AD61-4D284F264B60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{247A1E3C-87D8-467C-B97F-715594754AA3}"/>
+    <workbookView xWindow="2400" yWindow="3525" windowWidth="36000" windowHeight="14280" xr2:uid="{247A1E3C-87D8-467C-B97F-715594754AA3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -5290,8 +5290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4986B364-A491-49A2-9CB8-330D7C5C1208}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5406,16 +5406,16 @@
       <c r="F5">
         <v>0.48</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5">
         <v>0.54</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5">
         <v>0.84</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5">
         <v>0.47</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5">
         <v>0.6</v>
       </c>
     </row>
@@ -5572,8 +5572,12 @@
       <c r="H11">
         <v>1.07</v>
       </c>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
+      <c r="I11" s="4">
+        <v>0.63</v>
+      </c>
+      <c r="J11" s="4">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>

</xml_diff>

<commit_message>
update comparison plots, thicker traces, list of symbols
</commit_message>
<xml_diff>
--- a/Experiment/Analysis2.xlsx
+++ b/Experiment/Analysis2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\Documents\2023-FYP\Experiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D450F5F-8D4E-42F9-AD61-4D284F264B60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D887160-A0CD-45AF-9E12-BD2ABA0DA7CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2400" yWindow="3525" windowWidth="36000" windowHeight="14280" xr2:uid="{247A1E3C-87D8-467C-B97F-715594754AA3}"/>
   </bookViews>
@@ -316,16 +316,16 @@
                   <c:v>0.52</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.63</c:v>
+                  <c:v>0.67</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.71</c:v>
+                  <c:v>0.77</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.36</c:v>
+                  <c:v>0.35</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.63</c:v>
+                  <c:v>0.69</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -698,10 +698,10 @@
                   <c:v>0.89</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.52</c:v>
+                  <c:v>0.62</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.52</c:v>
+                  <c:v>0.78</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -798,16 +798,16 @@
                   <c:v>0.52</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.63</c:v>
+                  <c:v>0.67</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.71</c:v>
+                  <c:v>0.77</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.36</c:v>
+                  <c:v>0.35</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.63</c:v>
+                  <c:v>0.69</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1398,7 +1398,7 @@
                   <c:v>0.78</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.52</c:v>
+                  <c:v>0.62</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1475,7 +1475,7 @@
                   <c:v>0.89</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.52</c:v>
+                  <c:v>0.78</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1549,10 +1549,10 @@
                   <c:v>0.31</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.63</c:v>
+                  <c:v>0.67</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.36</c:v>
+                  <c:v>0.35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1626,10 +1626,10 @@
                   <c:v>0.52</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.71</c:v>
+                  <c:v>0.77</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.63</c:v>
+                  <c:v>0.69</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2297,10 +2297,10 @@
                   <c:v>0.89</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.52</c:v>
+                  <c:v>0.62</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.52</c:v>
+                  <c:v>0.78</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5291,7 +5291,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="I9" sqref="I9:J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5377,16 +5377,16 @@
         <v>0.52</v>
       </c>
       <c r="G4">
-        <v>0.63</v>
+        <v>0.67</v>
       </c>
       <c r="H4">
-        <v>0.71</v>
+        <v>0.77</v>
       </c>
       <c r="I4">
-        <v>0.36</v>
+        <v>0.35</v>
       </c>
       <c r="J4">
-        <v>0.63</v>
+        <v>0.69</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -5442,11 +5442,11 @@
       <c r="H6">
         <v>0.89</v>
       </c>
-      <c r="I6" s="1">
-        <v>0.52</v>
-      </c>
-      <c r="J6" s="1">
-        <v>0.52</v>
+      <c r="I6" s="4">
+        <v>0.62</v>
+      </c>
+      <c r="J6" s="4">
+        <v>0.78</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -5456,14 +5456,30 @@
       <c r="B7" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
+      <c r="C7" s="4">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0.33</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="G7" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="H7" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="I7" s="4">
+        <v>0.38</v>
+      </c>
+      <c r="J7" s="4">
+        <v>0.77</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
@@ -5572,10 +5588,10 @@
       <c r="H11">
         <v>1.07</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I11">
         <v>0.63</v>
       </c>
-      <c r="J11" s="4">
+      <c r="J11">
         <v>0.7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Circuit diagrams, internals, error table
</commit_message>
<xml_diff>
--- a/Experiment/Analysis2.xlsx
+++ b/Experiment/Analysis2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\Documents\2023-FYP\Experiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D887160-A0CD-45AF-9E12-BD2ABA0DA7CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74708966-4794-46BD-A8AF-7518EEEE09A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="3525" windowWidth="36000" windowHeight="14280" xr2:uid="{247A1E3C-87D8-467C-B97F-715594754AA3}"/>
+    <workbookView xWindow="2400" yWindow="3525" windowWidth="36000" windowHeight="14280" activeTab="1" xr2:uid="{247A1E3C-87D8-467C-B97F-715594754AA3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -152,14 +152,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5290,8 +5289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4986B364-A491-49A2-9CB8-330D7C5C1208}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9:J9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5442,10 +5441,10 @@
       <c r="H6">
         <v>0.89</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6">
         <v>0.62</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6">
         <v>0.78</v>
       </c>
     </row>
@@ -5456,28 +5455,28 @@
       <c r="B7" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7">
         <v>0.57999999999999996</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7">
         <v>0.57999999999999996</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7">
         <v>0.33</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7">
         <v>0.57999999999999996</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7">
         <v>0.7</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7">
         <v>0.75</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7">
         <v>0.38</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J7">
         <v>0.77</v>
       </c>
     </row>
@@ -5660,8 +5659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CD0A37E-004E-4ADA-86C5-3C95F5510AAC}">
   <dimension ref="B1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5737,16 +5736,16 @@
         <v>0.52</v>
       </c>
       <c r="G4">
-        <v>0.63</v>
+        <v>0.67</v>
       </c>
       <c r="H4">
-        <v>0.71</v>
+        <v>0.77</v>
       </c>
       <c r="I4">
-        <v>0.36</v>
+        <v>0.35</v>
       </c>
       <c r="J4">
-        <v>0.63</v>
+        <v>0.69</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
@@ -5765,17 +5764,17 @@
       <c r="F5">
         <v>0.48</v>
       </c>
-      <c r="G5" s="1">
-        <v>0.65</v>
-      </c>
-      <c r="H5" s="1">
-        <v>0.76</v>
-      </c>
-      <c r="I5" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="J5" s="1">
-        <v>0.57999999999999996</v>
+      <c r="G5">
+        <v>0.54</v>
+      </c>
+      <c r="H5">
+        <v>0.84</v>
+      </c>
+      <c r="I5">
+        <v>0.47</v>
+      </c>
+      <c r="J5">
+        <v>0.6</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
@@ -5800,11 +5799,11 @@
       <c r="H6">
         <v>0.89</v>
       </c>
-      <c r="I6" s="1">
-        <v>0.52</v>
-      </c>
-      <c r="J6" s="1">
-        <v>0.52</v>
+      <c r="I6">
+        <v>0.62</v>
+      </c>
+      <c r="J6">
+        <v>0.78</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
@@ -5878,19 +5877,19 @@
       </c>
       <c r="G12" s="2">
         <f t="shared" si="0"/>
-        <v>-0.19230769230769229</v>
+        <v>-0.14102564102564097</v>
       </c>
       <c r="H12" s="2">
         <f t="shared" si="0"/>
-        <v>-0.202247191011236</v>
+        <v>-0.1348314606741573</v>
       </c>
       <c r="I12" s="2">
         <f t="shared" si="0"/>
-        <v>-0.30769230769230771</v>
+        <v>-0.43548387096774199</v>
       </c>
       <c r="J12" s="2">
         <f t="shared" si="0"/>
-        <v>0.21153846153846145</v>
+        <v>-0.11538461538461553</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
@@ -5915,19 +5914,19 @@
       </c>
       <c r="G13" s="2">
         <f t="shared" si="1"/>
-        <v>-0.16666666666666663</v>
+        <v>-0.30769230769230771</v>
       </c>
       <c r="H13" s="2">
         <f t="shared" si="1"/>
-        <v>-0.1460674157303371</v>
+        <v>-5.6179775280898903E-2</v>
       </c>
       <c r="I13" s="2">
         <f t="shared" si="1"/>
-        <v>-3.8461538461538547E-2</v>
+        <v>-0.24193548387096775</v>
       </c>
       <c r="J13" s="2">
         <f t="shared" si="1"/>
-        <v>0.1153846153846152</v>
+        <v>-0.23076923076923084</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tail and mass plots
</commit_message>
<xml_diff>
--- a/Experiment/Analysis2.xlsx
+++ b/Experiment/Analysis2.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\Documents\2023-FYP\Experiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{673C816B-FAAC-4044-B0DA-33356E4C9058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EC1B900-6DBA-4AFB-BF50-DCB5B9F8ACB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30024" yWindow="2520" windowWidth="24600" windowHeight="14280" activeTab="1" xr2:uid="{247A1E3C-87D8-467C-B97F-715594754AA3}"/>
+    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{247A1E3C-87D8-467C-B97F-715594754AA3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2 (2)" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2 (3)" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="19">
   <si>
     <t>model</t>
   </si>
@@ -152,14 +154,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1288,11 +1289,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Torque</a:t>
+              <a:t>Experimental</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> required for partial movement</a:t>
+              <a:t> torque required</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -1337,7 +1338,15 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Experiment Partial</c:v>
+            <c:strRef>
+              <c:f>Sheet1!$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Experiment</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -1363,20 +1372,32 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>(Sheet1!$C$2,Sheet1!$E$2,Sheet1!$G$2,Sheet1!$I$2)</c:f>
+              <c:f>Sheet1!$C$2:$J$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
@@ -1384,21 +1405,33 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>(Sheet1!$C$6,Sheet1!$E$6,Sheet1!$G$6,Sheet1!$I$6)</c:f>
+              <c:f>Sheet1!$C$6:$J$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0.62</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.73</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.39</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>0.78</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
+                  <c:v>0.89</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.78</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1406,15 +1439,403 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-9175-41E2-9144-291C808BC2C5}"/>
+              <c16:uniqueId val="{00000000-F1A6-4E88-873F-95223A3E9778}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1845191072"/>
+        <c:axId val="1617548096"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1845191072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="7"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Stage of motion</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1617548096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1617548096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Torque [Nm]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1845191072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Torque</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> comparison with 60cm tail</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="3"/>
-          <c:order val="1"/>
+          <c:idx val="0"/>
+          <c:order val="0"/>
           <c:tx>
-            <c:v>Experiment Full</c:v>
+            <c:strRef>
+              <c:f>Sheet1!$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Experiment</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -1428,11 +1849,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent4"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent4"/>
+                  <a:schemeClr val="accent1"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -1440,20 +1861,32 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>(Sheet1!$D$2,Sheet1!$F$2,Sheet1!$H$2,Sheet1!$J$2)</c:f>
+              <c:f>Sheet1!$C$2:$J$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
@@ -1461,20 +1894,32 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>(Sheet1!$D$6,Sheet1!$F$6,Sheet1!$H$6,Sheet1!$J$6)</c:f>
+              <c:f>Sheet1!$C$9:$J$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.73</c:v>
+                  <c:v>0.71</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.39</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.89</c:v>
-                </c:pt>
                 <c:pt idx="3">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.61</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>0.78</c:v>
                 </c:pt>
               </c:numCache>
@@ -1483,15 +1928,23 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-9175-41E2-9144-291C808BC2C5}"/>
+              <c16:uniqueId val="{00000000-F2A8-48E4-BE3C-8D6061B8C409}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="2"/>
+          <c:order val="1"/>
           <c:tx>
-            <c:v>Model Partial</c:v>
+            <c:strRef>
+              <c:f>Sheet1!$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Model</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -1516,43 +1969,64 @@
             </c:spPr>
           </c:marker>
           <c:xVal>
-            <c:numRef>
-              <c:f>(Sheet1!$C$2,Sheet1!$E$2,Sheet1!$G$2,Sheet1!$I$2)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="8"/>
+              <c:pt idx="0">
+                <c:v>1.1000000000000001</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>1.1000000000000001</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>3.1</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>3.1</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>4.0999999999999899</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>4.0999999999999899</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>6.1</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>6.1</c:v>
+              </c:pt>
+            </c:numLit>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>(Sheet1!$C$4,Sheet1!$E$4,Sheet1!$G$4,Sheet1!$I$4)</c:f>
+              <c:f>Sheet1!$C$7:$J$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.52</c:v>
+                  <c:v>0.57999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.31</c:v>
+                  <c:v>0.57999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.67</c:v>
+                  <c:v>0.33</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.35</c:v>
+                  <c:v>0.57999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.77</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1560,92 +2034,23 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-9175-41E2-9144-291C808BC2C5}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:v>Model Full</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent5"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>(Sheet1!$D$2,Sheet1!$F$2,Sheet1!$H$2,Sheet1!$J$2)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>(Sheet1!$D$4,Sheet1!$F$4,Sheet1!$H$4,Sheet1!$J$4)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>0.52</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.52</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.77</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.69</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-9175-41E2-9144-291C808BC2C5}"/>
+              <c16:uniqueId val="{00000001-F2A8-48E4-BE3C-8D6061B8C409}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="4"/>
+          <c:order val="2"/>
           <c:tx>
-            <c:v>Simulation Partial</c:v>
+            <c:strRef>
+              <c:f>Sheet1!$B$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Simulation</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -1670,43 +2075,64 @@
             </c:spPr>
           </c:marker>
           <c:xVal>
-            <c:numRef>
-              <c:f>(Sheet1!$C$2,Sheet1!$E$2,Sheet1!$G$2,Sheet1!$I$2)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="8"/>
+              <c:pt idx="0">
+                <c:v>0.9</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>0.9</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>2.9</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>2.9</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>3.9</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>3.9</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>5.9</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>5.9</c:v>
+              </c:pt>
+            </c:numLit>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>(Sheet1!$C$5,Sheet1!$E$5,Sheet1!$G$5,Sheet1!$I$5)</c:f>
+              <c:f>Sheet1!$C$8:$J$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.53</c:v>
+                  <c:v>0.71</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.41</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.54</c:v>
+                  <c:v>0.56000000000000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.47</c:v>
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1714,84 +2140,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-9175-41E2-9144-291C808BC2C5}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:v>Simulation Full</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent6"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>(Sheet1!$D$2,Sheet1!$F$2,Sheet1!$H$2,Sheet1!$J$2)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>(Sheet1!$D$5,Sheet1!$F$5,Sheet1!$H$5,Sheet1!$J$5)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>0.68</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.48</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.84</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.59</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-9175-41E2-9144-291C808BC2C5}"/>
+              <c16:uniqueId val="{00000002-F2A8-48E4-BE3C-8D6061B8C409}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2123,7 +2472,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2158,11 +2507,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Experimental</a:t>
+              <a:t>Torque</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> torque required</a:t>
+              <a:t> comparison with 340g added mass</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -2274,33 +2623,33 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$6:$J$6</c:f>
+              <c:f>Sheet1!$C$12:$J$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.62</c:v>
+                  <c:v>0.84</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.73</c:v>
+                  <c:v>0.89</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.39</c:v>
+                  <c:v>0.47</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.39</c:v>
+                  <c:v>0.53</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.78</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.89</c:v>
+                  <c:v>1.26</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.62</c:v>
+                  <c:v>0.65</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.78</c:v>
+                  <c:v>0.91</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2308,7 +2657,219 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-F1A6-4E88-873F-95223A3E9778}"/>
+              <c16:uniqueId val="{00000000-A110-4C9A-8FED-F574DC5ACF76}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Model</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="8"/>
+              <c:pt idx="0">
+                <c:v>1.1000000000000001</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>1.1000000000000001</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>3.1</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>3.1</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>4.0999999999999899</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>4.0999999999999899</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>6.1</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>6.1</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$10:$J$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.37</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.1299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.99</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A110-4C9A-8FED-F574DC5ACF76}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Simulation</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="8"/>
+              <c:pt idx="0">
+                <c:v>0.9</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>0.9</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>2.9</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>2.9</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>3.9</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>3.9</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>5.9</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>5.9</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$11:$J$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.67</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.87</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.71</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.07</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.63</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-A110-4C9A-8FED-F574DC5ACF76}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2327,8 +2888,6 @@
         <c:axId val="1845191072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="7"/>
-          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -2441,7 +3000,6 @@
         <c:crossAx val="1617548096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="1617548096"/>
@@ -2568,6 +3126,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -2772,6 +3361,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -4836,20 +5465,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>392430</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>87630</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>87630</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>525780</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:rowOff>163830</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4876,16 +6021,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>609599</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>243839</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>123824</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>365759</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4907,44 +6052,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90FC4594-E0A6-4FAC-9D00-AF1E3C658A86}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4982,7 +6089,83 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>120015</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9AE5976E-FCD6-4EFA-A045-6CA4DD070CC7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>32385</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>148590</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>148590</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>110490</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89E41E81-F3C0-42C4-8BD2-D2AA087CD5F8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5290,8 +6473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4986B364-A491-49A2-9CB8-330D7C5C1208}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10:J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5415,7 +6598,7 @@
       <c r="I5">
         <v>0.47</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5">
         <v>0.59</v>
       </c>
     </row>
@@ -5504,10 +6687,10 @@
       <c r="H8">
         <v>0.85</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8">
         <v>0.48</v>
       </c>
-      <c r="J8" s="4">
+      <c r="J8">
         <v>0.6</v>
       </c>
     </row>
@@ -5534,8 +6717,12 @@
       <c r="H9">
         <v>0.95</v>
       </c>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
+      <c r="I9" s="1">
+        <v>0.61</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0.78</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
@@ -5622,7 +6809,9 @@
       <c r="H12">
         <v>1.26</v>
       </c>
-      <c r="I12" s="1"/>
+      <c r="I12" s="1">
+        <v>0.65</v>
+      </c>
       <c r="J12">
         <v>0.91</v>
       </c>
@@ -5664,8 +6853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CD0A37E-004E-4ADA-86C5-3C95F5510AAC}">
   <dimension ref="B1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5932,6 +7121,584 @@
       <c r="J13" s="2">
         <f t="shared" si="1"/>
         <v>-0.24358974358974361</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81E6C725-CA3B-48C4-B6D4-8E97C0E5D1FB}">
+  <dimension ref="B1:J13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:J6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3">
+        <v>3</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3">
+        <v>4</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3">
+        <v>6</v>
+      </c>
+      <c r="J2" s="3"/>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="D4">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="E4">
+        <v>0.33</v>
+      </c>
+      <c r="F4">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="G4">
+        <v>0.7</v>
+      </c>
+      <c r="H4">
+        <v>0.75</v>
+      </c>
+      <c r="I4">
+        <v>0.38</v>
+      </c>
+      <c r="J4">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>0.71</v>
+      </c>
+      <c r="D5">
+        <v>0.8</v>
+      </c>
+      <c r="E5">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="F5">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="G5">
+        <v>0.8</v>
+      </c>
+      <c r="H5">
+        <v>0.85</v>
+      </c>
+      <c r="I5">
+        <v>0.48</v>
+      </c>
+      <c r="J5">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>0.71</v>
+      </c>
+      <c r="D6">
+        <v>0.75</v>
+      </c>
+      <c r="E6">
+        <v>0.39</v>
+      </c>
+      <c r="F6">
+        <v>0.48</v>
+      </c>
+      <c r="G6">
+        <v>0.78</v>
+      </c>
+      <c r="H6">
+        <v>0.95</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0.61</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J10" s="3"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="2">
+        <f>C4/C6-1</f>
+        <v>-0.18309859154929575</v>
+      </c>
+      <c r="D12" s="2">
+        <f t="shared" ref="D12:J12" si="0">D4/D6-1</f>
+        <v>-0.22666666666666668</v>
+      </c>
+      <c r="E12" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.15384615384615385</v>
+      </c>
+      <c r="F12" s="2">
+        <f t="shared" si="0"/>
+        <v>0.20833333333333326</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.10256410256410264</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.21052631578947367</v>
+      </c>
+      <c r="I12" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.37704918032786883</v>
+      </c>
+      <c r="J12" s="2">
+        <f t="shared" si="0"/>
+        <v>-1.2820512820512886E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="2">
+        <f xml:space="preserve"> C5/C6-1</f>
+        <v>0</v>
+      </c>
+      <c r="D13" s="2">
+        <f t="shared" ref="D13:J13" si="1" xml:space="preserve"> D5/D6-1</f>
+        <v>6.6666666666666652E-2</v>
+      </c>
+      <c r="E13" s="2">
+        <f t="shared" si="1"/>
+        <v>0.4358974358974359</v>
+      </c>
+      <c r="F13" s="2">
+        <f t="shared" si="1"/>
+        <v>0.16666666666666674</v>
+      </c>
+      <c r="G13" s="2">
+        <f t="shared" si="1"/>
+        <v>2.5641025641025772E-2</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.10526315789473684</v>
+      </c>
+      <c r="I13" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.21311475409836067</v>
+      </c>
+      <c r="J13" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.23076923076923084</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{761CF769-29A2-4E21-9E1A-3645F1FC405C}">
+  <dimension ref="B1:J13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3">
+        <v>3</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3">
+        <v>4</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3">
+        <v>6</v>
+      </c>
+      <c r="J2" s="3"/>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>0.62</v>
+      </c>
+      <c r="D4">
+        <v>0.62</v>
+      </c>
+      <c r="E4">
+        <v>0.37</v>
+      </c>
+      <c r="F4">
+        <v>0.62</v>
+      </c>
+      <c r="G4">
+        <v>0.85</v>
+      </c>
+      <c r="H4">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="I4">
+        <v>0.45</v>
+      </c>
+      <c r="J4">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>0.67</v>
+      </c>
+      <c r="D5">
+        <v>0.87</v>
+      </c>
+      <c r="E5">
+        <v>0.52</v>
+      </c>
+      <c r="F5">
+        <v>0.6</v>
+      </c>
+      <c r="G5">
+        <v>0.71</v>
+      </c>
+      <c r="H5">
+        <v>1.07</v>
+      </c>
+      <c r="I5">
+        <v>0.63</v>
+      </c>
+      <c r="J5">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>0.84</v>
+      </c>
+      <c r="D6">
+        <v>0.89</v>
+      </c>
+      <c r="E6">
+        <v>0.47</v>
+      </c>
+      <c r="F6">
+        <v>0.53</v>
+      </c>
+      <c r="G6">
+        <v>0.9</v>
+      </c>
+      <c r="H6">
+        <v>1.26</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0.65</v>
+      </c>
+      <c r="J6">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J10" s="3"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="2">
+        <f>C4/C6-1</f>
+        <v>-0.26190476190476186</v>
+      </c>
+      <c r="D12" s="2">
+        <f t="shared" ref="D12:J12" si="0">D4/D6-1</f>
+        <v>-0.3033707865168539</v>
+      </c>
+      <c r="E12" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.21276595744680848</v>
+      </c>
+      <c r="F12" s="2">
+        <f t="shared" si="0"/>
+        <v>0.16981132075471694</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" si="0"/>
+        <v>-5.555555555555558E-2</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.10317460317460325</v>
+      </c>
+      <c r="I12" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.30769230769230771</v>
+      </c>
+      <c r="J12" s="2">
+        <f t="shared" si="0"/>
+        <v>8.7912087912087822E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="2">
+        <f xml:space="preserve"> C5/C6-1</f>
+        <v>-0.20238095238095233</v>
+      </c>
+      <c r="D13" s="2">
+        <f t="shared" ref="D13:J13" si="1" xml:space="preserve"> D5/D6-1</f>
+        <v>-2.2471910112359605E-2</v>
+      </c>
+      <c r="E13" s="2">
+        <f t="shared" si="1"/>
+        <v>0.1063829787234043</v>
+      </c>
+      <c r="F13" s="2">
+        <f t="shared" si="1"/>
+        <v>0.13207547169811318</v>
+      </c>
+      <c r="G13" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.21111111111111114</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.1507936507936507</v>
+      </c>
+      <c r="I13" s="2">
+        <f t="shared" si="1"/>
+        <v>-3.0769230769230771E-2</v>
+      </c>
+      <c r="J13" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.23076923076923084</v>
       </c>
     </row>
   </sheetData>

</xml_diff>